<commit_message>
fix "number" reference and add explicit test for bad types
</commit_message>
<xml_diff>
--- a/tests/012_ColumnsWithTypes.xlsx
+++ b/tests/012_ColumnsWithTypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">Data Source</t>
   </si>
@@ -67,7 +67,13 @@
     <t xml:space="preserve">a_number</t>
   </si>
   <si>
-    <t xml:space="preserve">number</t>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad_type</t>
   </si>
 </sst>
 </file>
@@ -179,21 +185,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1919642857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8526785714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7723214285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1964285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8035714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.8705357142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.71875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3794642857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8303571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7276785714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.2142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.9241071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,6 +258,17 @@
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>